<commit_message>
Merged in changes needed from other branches.
Files checked in: DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx DataRepo/management/commands/load_protocols.py DataRepo/models/maintained_model.py DataRepo/models/multi_db_mixin.py DataRepo/models/tracer_label.py DataRepo/templates/DataRepo/validate_submission.html DataRepo/templates/upload.html DataRepo/tests/loading/test_loading_protocols.py DataRepo/tests/test_queryset_to_dataframes.py DataRepo/tests/test_views.py DataRepo/utils/accucor_data_loader.py DataRepo/views/loading/validation.py DataRepo/models/infusate.py DataRepo/models/tracer.py DataRepo/utils/protocols_loader.py DataRepo/utils/sample_table_loader.py DataRepo/models/tracer_label.py
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_animal_and_sample_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcmatese/dev/tracebase/DataRepo/example_data/small_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/small_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0781DF80-725F-314E-A46A-292FFFD541A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EC9D00-BC86-984D-A0E7-8D8D048EAAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5640" yWindow="5120" windowWidth="29900" windowHeight="12800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,9 +474,6 @@
     <t>no treatment</t>
   </si>
   <si>
-    <t>No treatment was applied to the animal.  Animal was maintained on normal diet (LabDiet #5053 "Maintenance"), housed at room temperature with a normal light cycle.</t>
-  </si>
-  <si>
     <t>TraceBase Tissue Name</t>
   </si>
   <si>
@@ -818,6 +815,9 @@
   </si>
   <si>
     <t>ob/ob homozygouse mice were fasted</t>
+  </si>
+  <si>
+    <t>No manipulation besides what is already described in other fields.</t>
   </si>
 </sst>
 </file>
@@ -1253,13 +1253,13 @@
         <v>971</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="23">
         <v>26.3</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="23">
         <v>23.2</v>
@@ -1268,16 +1268,16 @@
         <v>0.11</v>
       </c>
       <c r="G2" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="23" t="s">
+      <c r="J2" s="23" t="s">
         <v>97</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
@@ -4347,16 +4347,16 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="23">
         <v>150</v>
@@ -4377,16 +4377,16 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D3" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="23">
         <v>150</v>
@@ -4407,16 +4407,16 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D4" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="23">
         <v>150</v>
@@ -4437,16 +4437,16 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D5" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="23">
         <v>150</v>
@@ -4467,16 +4467,16 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="23">
         <v>150</v>
@@ -4497,16 +4497,16 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D7" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="23">
         <v>150</v>
@@ -4527,16 +4527,16 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D8" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="23">
         <v>150</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D9" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="23">
         <v>150</v>
@@ -4587,16 +4587,16 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D10" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="23">
         <v>150</v>
@@ -4617,16 +4617,16 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="23">
         <v>150</v>
@@ -4647,16 +4647,16 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D12" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="23">
         <v>150</v>
@@ -4677,16 +4677,16 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D13" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="23">
         <v>150</v>
@@ -4707,16 +4707,16 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D14" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="23">
         <v>150</v>
@@ -4737,16 +4737,16 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D15" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="23">
         <v>150</v>
@@ -4767,16 +4767,16 @@
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>116</v>
-      </c>
       <c r="C16" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="23">
         <v>150</v>
@@ -4797,16 +4797,16 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D17" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="23">
         <v>150</v>
@@ -22560,7 +22560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -22606,15 +22606,15 @@
         <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -22644,10 +22644,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="7"/>
@@ -22675,295 +22675,295 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" ht="15">
+      <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:26" ht="15">
-      <c r="A3" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:26" ht="15">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" ht="15">
-      <c r="A4" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:26" ht="15">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:26" ht="15">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="1:26" ht="15">
+      <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:26" ht="15">
-      <c r="A6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:26" ht="15">
+      <c r="A7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:26" ht="15">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:26" ht="15">
+      <c r="A8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:26" ht="15">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:26" ht="15">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:26" ht="15">
-      <c r="A9" s="11" t="s">
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:26" ht="15">
+      <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:26" ht="15">
-      <c r="A10" s="11" t="s">
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:26" ht="15">
+      <c r="A11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:26" ht="15">
-      <c r="A11" s="11" t="s">
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:26" ht="15">
+      <c r="A12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:26" ht="15">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:26" ht="15">
+      <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:26" ht="15">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:26" ht="15">
+      <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:26" ht="15">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="11" t="s">
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="B16" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A17" s="15" t="s">
+      <c r="B17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="11" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A18" s="15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
+      <c r="B18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="11" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="11" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A21" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="11" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A22" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="11" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A23" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="B23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="15" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="B24" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="11" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A26" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="11" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="B27" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A28" s="11" t="s">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A29" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A29" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="11" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A30" s="11" t="s">
+      <c r="B30" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="11" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A31" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A31" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="11" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A32" s="11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
+      <c r="B32" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="15" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="B33" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A34" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B34" s="15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="11" t="s">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A35" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A35" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="11" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A36" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A36" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -23015,76 +23015,76 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="19" t="s">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A5" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="19" t="s">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A6" s="19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="19" t="s">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="19" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="19" t="s">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:26" ht="18">
       <c r="A17" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -23114,22 +23114,22 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A19" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A20" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>